<commit_message>
Finally got my solution working
The key is understanding that SUMIF seems to struggle in these array expressions, but SUM with FILTER does just fine.
</commit_message>
<xml_diff>
--- a/CH-044 Combine Tables.xlsx
+++ b/CH-044 Combine Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{64C55396-FB45-492D-B9BD-78BE557FF50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FDEBF2-0931-4FC7-ADC6-BC2228979980}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{64C55396-FB45-492D-B9BD-78BE557FF50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1E88C86-6113-47E4-A3BB-40E640234532}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="43">
   <si>
     <t>Product A</t>
   </si>
@@ -142,12 +142,60 @@
   <si>
     <t>Columns to take</t>
   </si>
+  <si>
+    <t>Let's explore the F utility.</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Region 1Product A</t>
+  </si>
+  <si>
+    <t>Lesssons</t>
+  </si>
+  <si>
+    <t>IFS(A,A) can be used to select text</t>
+  </si>
+  <si>
+    <t>My Solution</t>
+  </si>
+  <si>
+    <t>SUMIFS is a problem in these array formulas, but SUM works fine</t>
+  </si>
+  <si>
+    <t>when coupled with FILTER</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +243,13 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -271,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -423,12 +478,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -483,12 +554,36 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3362,10 +3457,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0520B225-0DE8-4C5E-8F61-2E80D05807A8}">
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="N56" sqref="N55:N56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74:C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3375,7 +3470,7 @@
     <col min="3" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="18.5546875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
     <col min="9" max="9" width="6.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
     <col min="11" max="13" width="10.109375" customWidth="1"/>
@@ -3840,12 +3935,11 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F26" s="22" t="str" cm="1">
-        <f t="array" ref="F26:H37">_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C10:C12&amp;"|"&amp;D9:G9),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D10:G12))</f>
-        <v>Region 1</v>
-      </c>
-      <c r="G26" s="22" t="str">
-        <v>Product A</v>
+      <c r="F26" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>0</v>
       </c>
       <c r="H26" s="22">
         <v>90</v>
@@ -3876,11 +3970,11 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F27" s="22" t="str">
-        <v>Region 1</v>
-      </c>
-      <c r="G27" s="22" t="str">
-        <v>Product D</v>
+      <c r="F27" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>9</v>
       </c>
       <c r="H27" s="22">
         <v>30</v>
@@ -3910,11 +4004,11 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F28" s="22" t="str">
-        <v>Region 1</v>
-      </c>
-      <c r="G28" s="22" t="str">
-        <v>Product C</v>
+      <c r="F28" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>2</v>
       </c>
       <c r="H28" s="22">
         <v>95</v>
@@ -3944,11 +4038,11 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F29" s="22" t="str">
-        <v>Region 1</v>
-      </c>
-      <c r="G29" s="22" t="str">
-        <v>Product E</v>
+      <c r="F29" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="H29" s="22">
         <v>74</v>
@@ -3978,33 +4072,33 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F30" s="22" t="str">
-        <v>Region 4</v>
-      </c>
-      <c r="G30" s="22" t="str">
-        <v>Product A</v>
+      <c r="F30" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>0</v>
       </c>
       <c r="H30" s="22">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F31" s="22" t="str">
-        <v>Region 4</v>
-      </c>
-      <c r="G31" s="22" t="str">
-        <v>Product D</v>
+      <c r="F31" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>9</v>
       </c>
       <c r="H31" s="22">
         <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F32" s="22" t="str">
-        <v>Region 4</v>
-      </c>
-      <c r="G32" s="22" t="str">
-        <v>Product C</v>
+      <c r="F32" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>2</v>
       </c>
       <c r="H32" s="22">
         <v>80</v>
@@ -4029,12 +4123,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F33" s="22" t="str">
-        <v>Region 4</v>
-      </c>
-      <c r="G33" s="22" t="str">
-        <v>Product E</v>
+    <row r="33" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F33" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="H33" s="22">
         <v>17</v>
@@ -4058,12 +4152,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F34" s="22" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G34" s="22" t="str">
-        <v>Product A</v>
+    <row r="34" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F34" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>0</v>
       </c>
       <c r="H34" s="22">
         <v>88</v>
@@ -4087,12 +4181,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F35" s="22" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G35" s="22" t="str">
-        <v>Product D</v>
+    <row r="35" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F35" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>9</v>
       </c>
       <c r="H35" s="22">
         <v>37</v>
@@ -4116,12 +4210,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F36" s="22" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G36" s="22" t="str">
-        <v>Product C</v>
+    <row r="36" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F36" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>2</v>
       </c>
       <c r="H36" s="22">
         <v>69</v>
@@ -4145,35 +4239,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F37" s="22" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G37" s="22" t="str">
-        <v>Product E</v>
+    <row r="37" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F37" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="H37" s="22">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F38" s="23" t="str" cm="1">
-        <f t="array" ref="F38:H46">_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C4:C6&amp;"|"&amp;D3:F3),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D4:F6))</f>
-        <v>Region 1</v>
-      </c>
-      <c r="G38" s="23" t="str">
-        <v>Product A</v>
+    <row r="38" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F38" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>0</v>
       </c>
       <c r="H38" s="23">
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F39" s="23" t="str">
-        <v>Region 1</v>
-      </c>
-      <c r="G39" s="23" t="str">
-        <v>Product B</v>
+    <row r="39" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F39" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="23" t="s">
+        <v>1</v>
       </c>
       <c r="H39" s="23">
         <v>45</v>
@@ -4183,12 +4276,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="40" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F40" s="23" t="str">
-        <v>Region 1</v>
-      </c>
-      <c r="G40" s="23" t="str">
-        <v>Product E</v>
+    <row r="40" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F40" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="H40" s="23">
         <v>91</v>
@@ -4197,12 +4290,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F41" s="23" t="str">
-        <v>Region 2</v>
-      </c>
-      <c r="G41" s="23" t="str">
-        <v>Product A</v>
+    <row r="41" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F41" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>0</v>
       </c>
       <c r="H41" s="23">
         <v>37</v>
@@ -4211,12 +4304,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F42" s="23" t="str">
-        <v>Region 2</v>
-      </c>
-      <c r="G42" s="23" t="str">
-        <v>Product B</v>
+    <row r="42" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F42" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>1</v>
       </c>
       <c r="H42" s="23">
         <v>71</v>
@@ -4225,161 +4318,172 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F43" s="23" t="str">
-        <v>Region 2</v>
-      </c>
-      <c r="G43" s="23" t="str">
-        <v>Product E</v>
+    <row r="43" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F43" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="H43" s="23">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F44" s="23" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G44" s="23" t="str">
-        <v>Product A</v>
+    <row r="44" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F44" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="23" t="s">
+        <v>0</v>
       </c>
       <c r="H44" s="23">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F45" s="23" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G45" s="23" t="str">
-        <v>Product B</v>
+    <row r="45" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F45" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="23" t="s">
+        <v>1</v>
       </c>
       <c r="H45" s="23">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F46" s="23" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G46" s="23" t="str">
-        <v>Product E</v>
+    <row r="46" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F46" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="H46" s="23">
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F47" s="24" t="str" cm="1">
-        <f t="array" ref="F47:H55">_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C16:C18&amp;"|"&amp;D15:F15),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D16:F18))</f>
-        <v>Region 3</v>
-      </c>
-      <c r="G47" s="24" t="str">
-        <v>Product D</v>
+    <row r="47" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F47" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="H47" s="24">
         <v>77</v>
       </c>
-    </row>
-    <row r="48" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F48" s="24" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G48" s="24" t="str">
-        <v>Product B</v>
+      <c r="U47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="F48" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>1</v>
       </c>
       <c r="H48" s="24">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F49" s="24" t="str">
-        <v>Region 3</v>
-      </c>
-      <c r="G49" s="24" t="str">
-        <v>Product E</v>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F49" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>10</v>
       </c>
       <c r="H49" s="24">
         <v>37</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F50" s="24" t="str">
-        <v>Region 2</v>
-      </c>
-      <c r="G50" s="24" t="str">
-        <v>Product D</v>
+      <c r="U49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F50" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="H50" s="24">
         <v>98</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F51" s="24" t="str">
-        <v>Region 2</v>
-      </c>
-      <c r="G51" s="24" t="str">
-        <v>Product B</v>
+      <c r="U50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F51" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>1</v>
       </c>
       <c r="H51" s="24">
         <v>66</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F52" s="24" t="str">
-        <v>Region 2</v>
-      </c>
-      <c r="G52" s="24" t="str">
-        <v>Product E</v>
+      <c r="U51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F52" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>10</v>
       </c>
       <c r="H52" s="24">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F53" s="24" t="str">
-        <v>Region 4</v>
-      </c>
-      <c r="G53" s="24" t="str">
-        <v>Product D</v>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F53" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="H53" s="24">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F54" s="24" t="str">
-        <v>Region 4</v>
-      </c>
-      <c r="G54" s="24" t="str">
-        <v>Product B</v>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F54" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="24" t="s">
+        <v>1</v>
       </c>
       <c r="H54" s="24">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F55" s="24" t="str">
-        <v>Region 4</v>
-      </c>
-      <c r="G55" s="24" t="str">
-        <v>Product E</v>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F55" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="24" t="s">
+        <v>10</v>
       </c>
       <c r="H55" s="24">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="O56" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C60" s="29" t="str" cm="1">
         <f t="array" ref="C60:H64">_xlfn.LET(_xlpm.u,_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C10:C12&amp;"|"&amp;D9:G9),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D10:G12)),
 _xlpm.m,_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C4:C6&amp;"|"&amp;D3:F3),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D4:F6)),
@@ -4387,7 +4491,7 @@
 _xlpm.q,_xlfn.VSTACK(_xlpm.u,_xlpm.m,_xlpm.l),
 _xlpm.tt, _xlfn.CHOOSECOLS(_xlpm.q,3),
 _xlpm.tc,_xlfn._xlws.SORT(TRANSPOSE(_xlfn.UNIQUE(G26:G55)),1,1,TRUE),
-_xlpm.lh,_xlfn._xlws.SORT(_xlfn.UNIQUE(F26:F55)),
+_xlpm.lh,_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.TAKE(_xlpm.q,,1))),
 _xlpm.zz,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.tc,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,SUMIFS(H26:H55,F26:F55,_xlpm.lh,G26:G55,_xlpm.v)))),,1),
 _xlfn.HSTACK(_xlfn.VSTACK("Regions",_xlpm.lh),_xlfn.VSTACK(_xlpm.tc,_xlpm.zz))
 )</f>
@@ -4409,7 +4513,7 @@
         <v>Product E</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C61" s="27" t="str">
         <v>Region 1</v>
       </c>
@@ -4429,7 +4533,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C62" s="27" t="str">
         <v>Region 2</v>
       </c>
@@ -4449,7 +4553,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C63" s="27" t="str">
         <v>Region 3</v>
       </c>
@@ -4469,7 +4573,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C64" s="27" t="str">
         <v>Region 4</v>
       </c>
@@ -4489,60 +4593,285 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C67" cm="1">
-        <f t="array" ref="C67:G67">_xlfn.LET(_xlpm.u,_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C10:C12&amp;"|"&amp;D9:G9),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D10:G12)),
-_xlpm.m,_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C4:C6&amp;"|"&amp;D3:F3),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D4:F6)),
-_xlpm.l,_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C16:C18&amp;"|"&amp;D15:F15),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D16:F18)),
-_xlpm.q,_xlfn.VSTACK(_xlpm.u,_xlpm.m,_xlpm.l),
-_xlpm.tt_, _xlfn.CHOOSECOLS(_xlpm.q,2),
-_xlpm.tc,_xlfn._xlws.SORT(TRANSPOSE(_xlfn.UNIQUE(G26:G55)),1,1,TRUE),
-_xlpm.lh,_xlfn._xlws.SORT(_xlfn.UNIQUE(F26:F55)),
-_xlpm.zz,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.tc,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,SUM(_xlfn.TAKE(_xlfn._xlws.FILTER(_xlpm.q,_xlfn.CHOOSECOLS(_xlpm.q,2)=_xlpm.v),,-1))))),,1),
-_xlpm.zz
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A66" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C68" s="33" t="str" cm="1">
+        <f t="array" ref="C68:H72">_xlfn.LET(_xlpm.u,_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C10:C12&amp;"|"&amp;D9:G9),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D10:G12)),
+     _xlpm.m,_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C4:C6&amp;"|"&amp;D3:F3),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D4:F6)),
+     _xlpm.l,_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TOCOL(C16:C18&amp;"|"&amp;D15:F15),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1),_xlfn.TOCOL(D16:F18)),
+     _xlpm.q,_xlfn.VSTACK(_xlpm.u,_xlpm.m,_xlpm.l),
+     _xlpm.tc,_xlfn._xlws.SORT(TRANSPOSE(_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.q,2))),1,1,TRUE),
+     _xlpm.lh,_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.q,1))),
+     _xlpm.zz,_xlfn.MAP(_xlpm.lh&amp;_xlpm.tc,_xlfn.LAMBDA(_xlpm.x,SUM(_xlfn._xlws.FILTER(_xlpm.q,_xlfn.CHOOSECOLS(_xlpm.q,1)&amp;_xlfn.CHOOSECOLS(_xlpm.q,2)=_xlpm.x,0)))),
+     _xlfn.HSTACK(_xlfn.VSTACK("Regions",_xlpm.lh),_xlfn.VSTACK(_xlpm.tc,_xlpm.zz))
 )</f>
-        <v>456</v>
-      </c>
-      <c r="D67">
-        <v>300</v>
-      </c>
-      <c r="E67">
-        <v>244</v>
-      </c>
-      <c r="F67">
-        <v>315</v>
-      </c>
-      <c r="G67">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A70" s="21" t="s">
+        <v>Regions</v>
+      </c>
+      <c r="D68" s="36" t="str">
+        <v>Product A</v>
+      </c>
+      <c r="E68" s="36" t="str">
+        <v>Product B</v>
+      </c>
+      <c r="F68" s="34" t="str">
+        <v>Product C</v>
+      </c>
+      <c r="G68" s="36" t="str">
+        <v>Product D</v>
+      </c>
+      <c r="H68" s="36" t="str">
+        <v>Product E</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C69" s="37" t="str">
+        <v>Region 1</v>
+      </c>
+      <c r="D69" s="35">
+        <v>188</v>
+      </c>
+      <c r="E69" s="35">
+        <v>45</v>
+      </c>
+      <c r="F69" s="35">
+        <v>95</v>
+      </c>
+      <c r="G69" s="35">
+        <v>30</v>
+      </c>
+      <c r="H69" s="35">
+        <v>165</v>
+      </c>
+      <c r="J69" t="str" cm="1">
+        <f t="array" ref="J69:L70">_xlfn.LET(_xlpm.q, F26:H55, _xlfn._xlws.FILTER(_xlpm.q,_xlfn.CHOOSECOLS(_xlpm.q,1)&amp;_xlfn.CHOOSECOLS(_xlpm.q,2)="Region 4Product D",0))</f>
+        <v>Region 4</v>
+      </c>
+      <c r="K69" t="str">
+        <v>Product D</v>
+      </c>
+      <c r="L69">
+        <v>41</v>
+      </c>
+      <c r="N69" s="7" t="str" cm="1">
+        <f t="array" ref="N69:N98">_xlfn.LET(_xlpm.q, F26:H55,_xlfn.CHOOSECOLS(_xlpm.q,1)&amp;_xlfn.CHOOSECOLS(_xlpm.q,2))</f>
+        <v>Region 1Product A</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C70" s="37" t="str">
+        <v>Region 2</v>
+      </c>
+      <c r="D70" s="35">
+        <v>37</v>
+      </c>
+      <c r="E70" s="35">
+        <v>137</v>
+      </c>
+      <c r="F70" s="35">
+        <v>0</v>
+      </c>
+      <c r="G70" s="35">
+        <v>98</v>
+      </c>
+      <c r="H70" s="35">
+        <v>82</v>
+      </c>
+      <c r="J70" t="str">
+        <v>Region 4</v>
+      </c>
+      <c r="K70" t="str">
+        <v>Product D</v>
+      </c>
+      <c r="L70">
+        <v>32</v>
+      </c>
+      <c r="N70" s="7" t="str">
+        <v>Region 1Product D</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C71" s="37" t="str">
+        <v>Region 3</v>
+      </c>
+      <c r="D71" s="35">
+        <v>180</v>
+      </c>
+      <c r="E71" s="35">
+        <v>61</v>
+      </c>
+      <c r="F71" s="35">
+        <v>69</v>
+      </c>
+      <c r="G71" s="35">
+        <v>114</v>
+      </c>
+      <c r="H71" s="35">
+        <v>197</v>
+      </c>
+      <c r="N71" s="7" t="str">
+        <v>Region 1Product C</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C72" s="37" t="str">
+        <v>Region 4</v>
+      </c>
+      <c r="D72" s="35">
+        <v>51</v>
+      </c>
+      <c r="E72" s="35">
+        <v>57</v>
+      </c>
+      <c r="F72" s="35">
+        <v>80</v>
+      </c>
+      <c r="G72" s="35">
+        <v>73</v>
+      </c>
+      <c r="H72" s="35">
+        <v>46</v>
+      </c>
+      <c r="N72" s="7" t="str">
+        <v>Region 1Product E</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N73" s="7" t="str">
+        <v>Region 4Product A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N74" s="7" t="str">
+        <v>Region 4Product D</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N75" s="7" t="str">
+        <v>Region 4Product C</v>
+      </c>
+      <c r="T75" t="s">
+        <v>28</v>
+      </c>
+      <c r="U75">
+        <v>1</v>
+      </c>
+      <c r="V75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N76" s="7" t="str">
+        <v>Region 4Product E</v>
+      </c>
+      <c r="T76">
+        <v>3</v>
+      </c>
+      <c r="U76" t="s">
+        <v>29</v>
+      </c>
+      <c r="V76" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N77" s="7" t="str">
+        <v>Region 3Product A</v>
+      </c>
+      <c r="T77">
+        <v>4</v>
+      </c>
+      <c r="U77">
+        <v>5</v>
+      </c>
+      <c r="V77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N78" s="7" t="str">
+        <v>Region 3Product D</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N79" s="7" t="str">
+        <v>Region 3Product C</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N80" s="7" t="str">
+        <v>Region 3Product E</v>
+      </c>
+      <c r="T80" t="e" cm="1">
+        <f t="array" ref="T80:V82">_xlfn.IFS(T75:V77,T75:V77)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U80">
+        <v>1</v>
+      </c>
+      <c r="V80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A81" s="21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C72" t="str" cm="1">
-        <f t="array" ref="C72:H76">_xlfn.LET(_xlpm.A, C3:F6, _xlpm.B, C9:G12, _xlpm.C, C15:F18, _xlpm.F, _xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z, _xlfn.DROP(_xlfn.UNIQUE(_xlfn.TAKE(_xlpm.x, _xlpm.y, _xlpm.z), _xlpm.y), _xlpm.z, _xlpm.y)), _xlpm.P, _xlpm.F(_xlfn.HSTACK(_xlpm.A,_xlpm.B,_xlpm.C),1,), _xlpm.R, _xlpm.F(_xlfn.VSTACK(_xlpm.A,_xlpm.B,_xlpm.C),,1), _xlpm.G, _xlfn.LAMBDA(_xlpm.i, _xlfn.XLOOKUP(_xlpm.R&amp;_xlfn.SORTBY(_xlpm.P, RIGHT(_xlpm.P)), _xlfn.TOCOL(_xlpm.F(_xlpm.i,,1)&amp;_xlpm.F(_xlpm.i,1,)), _xlfn.TOCOL(_xlfn.IFS(_xlpm.i, _xlpm.i), 2), 0)), _xlfn.VSTACK(_xlfn.HSTACK(C3,_xlfn.SORTBY(_xlpm.P,RIGHT(_xlpm.P))),_xlfn.HSTACK(_xlpm.R,_xlpm.G(_xlpm.A)+_xlpm.G(_xlpm.B)+_xlpm.G(_xlpm.C))))</f>
+      <c r="N81" s="7" t="str">
+        <v>Region 1Product A</v>
+      </c>
+      <c r="T81">
+        <v>3</v>
+      </c>
+      <c r="U81" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="V81" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N82" s="7" t="str">
+        <v>Region 1Product B</v>
+      </c>
+      <c r="T82">
+        <v>4</v>
+      </c>
+      <c r="U82">
+        <v>5</v>
+      </c>
+      <c r="V82" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C83" t="str" cm="1">
+        <f t="array" ref="C83:H87">_xlfn.LET(_xlpm.A, C3:F6, _xlpm.B, C9:G12, _xlpm.C, C15:F18, _xlpm.F, _xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z, _xlfn.DROP(_xlfn.UNIQUE(_xlfn.TAKE(_xlpm.x, _xlpm.y, _xlpm.z), _xlpm.y), _xlpm.z, _xlpm.y)), _xlpm.P, _xlpm.F(_xlfn.HSTACK(_xlpm.A,_xlpm.B,_xlpm.C),1,), _xlpm.R, _xlpm.F(_xlfn.VSTACK(_xlpm.A,_xlpm.B,_xlpm.C),,1), _xlpm.G, _xlfn.LAMBDA(_xlpm.i, _xlfn.XLOOKUP(_xlpm.R&amp;_xlfn.SORTBY(_xlpm.P, RIGHT(_xlpm.P)), _xlfn.TOCOL(_xlpm.F(_xlpm.i,,1)&amp;_xlpm.F(_xlpm.i,1,)), _xlfn.TOCOL(_xlfn.IFS(_xlpm.i, _xlpm.i), 2), 0)), _xlfn.VSTACK(_xlfn.HSTACK(C3,_xlfn.SORTBY(_xlpm.P,RIGHT(_xlpm.P))),_xlfn.HSTACK(_xlpm.R,_xlpm.G(_xlpm.A)+_xlpm.G(_xlpm.B)+_xlpm.G(_xlpm.C))))</f>
         <v>Regions</v>
       </c>
-      <c r="D72" t="str">
+      <c r="D83" t="str">
         <v>Product A</v>
       </c>
-      <c r="E72" t="str">
+      <c r="E83" t="str">
         <v>Product B</v>
       </c>
-      <c r="F72" s="7" t="str">
+      <c r="F83" s="7" t="str">
         <v>Product C</v>
       </c>
-      <c r="G72" t="str">
+      <c r="G83" t="str">
         <v>Product D</v>
       </c>
-      <c r="H72" t="str">
+      <c r="H83" t="str">
         <v>Product E</v>
       </c>
-      <c r="J72" cm="1">
-        <f t="array" ref="J72:J80">_xlfn.LET(_xlpm.A, C3:F6,
+      <c r="J83" cm="1">
+        <f t="array" ref="J83:J91">_xlfn.LET(_xlpm.A, C3:F6,
      _xlpm.B, C9:G12,
      _xlpm.C, C15:F18,
      _xlpm.F, _xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z, _xlfn.DROP(_xlfn.UNIQUE(_xlfn.TAKE(_xlpm.x, _xlpm.y, _xlpm.z), _xlpm.y), _xlpm.z, _xlpm.y)),
@@ -4552,147 +4881,248 @@
      _xlfn.TOCOL(_xlfn.IFS(_xlpm.A,_xlpm.A),2))</f>
         <v>98</v>
       </c>
-      <c r="N72"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C73" t="str">
+      <c r="N83" t="str">
+        <v>Region 1Product E</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C84" t="str">
         <v>Region 1</v>
       </c>
-      <c r="D73">
+      <c r="D84">
         <v>188</v>
       </c>
-      <c r="E73">
+      <c r="E84">
         <v>45</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F84" s="7">
         <v>95</v>
       </c>
-      <c r="G73">
+      <c r="G84">
         <v>30</v>
       </c>
-      <c r="H73">
+      <c r="H84">
         <v>165</v>
       </c>
-      <c r="J73">
+      <c r="J84">
         <v>45</v>
       </c>
-      <c r="N73"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C74" t="str">
+      <c r="N84" t="str">
+        <v>Region 2Product A</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C85" t="str">
         <v>Region 2</v>
       </c>
-      <c r="D74">
+      <c r="D85">
         <v>37</v>
       </c>
-      <c r="E74">
+      <c r="E85">
         <v>137</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F85" s="7">
         <v>0</v>
       </c>
-      <c r="G74">
+      <c r="G85">
         <v>98</v>
       </c>
-      <c r="H74">
+      <c r="H85">
         <v>82</v>
       </c>
-      <c r="J74">
+      <c r="J85">
         <v>91</v>
       </c>
-      <c r="N74"/>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C75" t="str">
+      <c r="N85" t="str">
+        <v>Region 2Product B</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C86" t="str">
         <v>Region 3</v>
       </c>
-      <c r="D75">
+      <c r="D86">
         <v>180</v>
       </c>
-      <c r="E75">
+      <c r="E86">
         <v>61</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F86" s="7">
         <v>69</v>
       </c>
-      <c r="G75">
+      <c r="G86">
         <v>114</v>
       </c>
-      <c r="H75">
+      <c r="H86">
         <v>197</v>
       </c>
-      <c r="J75">
+      <c r="J86">
         <v>37</v>
       </c>
-      <c r="N75"/>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C76" t="str">
+      <c r="N86" t="str">
+        <v>Region 2Product E</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C87" t="str">
         <v>Region 4</v>
       </c>
-      <c r="D76">
+      <c r="D87">
         <v>51</v>
       </c>
-      <c r="E76">
+      <c r="E87">
         <v>57</v>
       </c>
-      <c r="F76" s="7">
+      <c r="F87" s="7">
         <v>80</v>
       </c>
-      <c r="G76">
+      <c r="G87">
         <v>73</v>
       </c>
-      <c r="H76">
+      <c r="H87">
         <v>46</v>
       </c>
-      <c r="J76">
+      <c r="J87">
         <v>71</v>
       </c>
-      <c r="N76"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J77">
+      <c r="N87" t="str">
+        <v>Region 3Product A</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J88">
         <v>23</v>
       </c>
-      <c r="M77" t="s">
+      <c r="N88" s="7" t="str">
+        <v>Region 3Product B</v>
+      </c>
+      <c r="S88" t="s">
         <v>20</v>
       </c>
-      <c r="N77"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J78">
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J89">
         <v>92</v>
       </c>
-      <c r="N78"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J79">
+      <c r="N89" s="7" t="str">
+        <v>Region 3Product E</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J90">
         <v>39</v>
       </c>
-      <c r="M79" t="s">
+      <c r="N90" s="7" t="str">
+        <v>Region 3Product D</v>
+      </c>
+      <c r="S90" t="s">
         <v>21</v>
       </c>
-      <c r="N79" t="s">
+      <c r="T90" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J80">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J91">
         <v>90</v>
       </c>
-      <c r="M80" t="s">
+      <c r="N91" s="7" t="str">
+        <v>Region 3Product B</v>
+      </c>
+      <c r="S91" t="s">
         <v>23</v>
       </c>
-      <c r="N80" t="s">
+      <c r="T91" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="13:14" x14ac:dyDescent="0.3">
-      <c r="M81" t="s">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N92" s="7" t="str">
+        <v>Region 3Product E</v>
+      </c>
+      <c r="S92" t="s">
         <v>25</v>
       </c>
-      <c r="N81" t="s">
+      <c r="T92" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N93" s="7" t="str">
+        <v>Region 2Product D</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N94" s="7" t="str">
+        <v>Region 2Product B</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N95" s="7" t="str">
+        <v>Region 2Product E</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>27</v>
+      </c>
+      <c r="N96" s="7" t="str">
+        <v>Region 4Product D</v>
+      </c>
+    </row>
+    <row r="97" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="N97" s="7" t="str">
+        <v>Region 4Product B</v>
+      </c>
+    </row>
+    <row r="98" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C98" t="str" cm="1">
+        <f t="array" ref="C98:C100">_xlfn.LET(_xlpm.A,C15:F18,
+     _xlpm.F, _xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z, _xlfn.DROP(_xlfn.UNIQUE(_xlfn.TAKE(_xlpm.x, _xlpm.y, _xlpm.z), _xlpm.y), _xlpm.z, _xlpm.y)),
+     _xlpm.F(_xlpm.A,,1))</f>
+        <v>Region 3</v>
+      </c>
+      <c r="N98" s="7" t="str">
+        <v>Region 4Product E</v>
+      </c>
+    </row>
+    <row r="99" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C99" t="str">
+        <v>Region 2</v>
+      </c>
+      <c r="F99" t="s">
+        <v>28</v>
+      </c>
+      <c r="G99" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C100" t="str">
+        <v>Region 4</v>
+      </c>
+      <c r="F100" t="s">
+        <v>31</v>
+      </c>
+      <c r="G100" t="s">
+        <v>32</v>
+      </c>
+      <c r="H100" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F101" t="s">
+        <v>34</v>
+      </c>
+      <c r="G101" t="s">
+        <v>35</v>
+      </c>
+      <c r="H101" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>